<commit_message>
readme file, env and dockerfile adjustments
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ubuntu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DA2DFE-FE1D-44F0-BCDA-4E72B6B452D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1324B0-AF55-4543-A9AF-B3654CAEE0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11268" yWindow="684" windowWidth="11568" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>https://storage-api.petstory.ru/resize/1000x1000x80/cb/48/7f/cb487f4677a640329e92ac0076004607.jpeg</t>
   </si>
   <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcREP-2PQjn2LO8mzNybmzJpt3C7e2rV1eTUmw&amp;s</t>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQaMN6ffiE9VmrBh5g0fq8qyvXZGfpQg3D2vA&amp;s</t>
   </si>
   <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQaMN6ffiE9VmrBh5g0fq8qyvXZGfpQg3D2vA&amp;s</t>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ2DojOyfbjvs8IDSMwA3TnZZuPAheTa22qkw&amp;s</t>
+  </si>
+  <si>
+    <t>https://www.ferra.ru/imgs/2022/02/01/15/5208913/95814d9ab375488468e6df2d5d74b98be7af0bee.webp</t>
   </si>
 </sst>
 </file>
@@ -362,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -377,12 +380,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -390,6 +398,7 @@
     <hyperlink ref="A1" r:id="rId1" xr:uid="{F938D1EC-0AFB-414C-84A7-E753DDAB8931}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{9C88E56E-0A4A-40CB-89F8-156CEC736A38}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{D0E9E38B-836B-4C25-8C28-AD982693D04F}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{725FA3DA-9BA8-42B5-B71A-65A6A95AF09C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>